<commit_message>
Adiciona arquivos e planilhas locais ao projeto
</commit_message>
<xml_diff>
--- a/data/processed/Planilha_Artigos_Automatizada.xlsx
+++ b/data/processed/Planilha_Artigos_Automatizada.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b762d1a876c02ea/Pessoal - UFG/MESTRADO/EVENTOS/ENIPAC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b762d1a876c02ea/Pessoal - UFG/MESTRADO/EVENTOS/ENIPAC/smart-heritage-review/smart-heritage-review/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_F56E7CDDF13129FBA4160B2F9B9AD6DB502E69BB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC722568-F511-4CD0-8911-B345C65A5916}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_F56E7CDDF13129FBA4160B2F9B9AD6DB502E69BB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{493A2F33-3828-41E6-B058-F05607C218B9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$170</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="860">
   <si>
     <t>ID_Zotero</t>
   </si>
@@ -1081,42 +1084,21 @@
     <t>Tunísia</t>
   </si>
   <si>
-    <t>Dispilio é uma antiga aldeia lacustre pré-histórica localizada na Grécia.</t>
-  </si>
-  <si>
     <t>China</t>
   </si>
   <si>
-    <t>São Paulo, Brasil.</t>
-  </si>
-  <si>
     <t>Irã</t>
   </si>
   <si>
-    <t>Santiago de los Caballeros, República Dominicana.</t>
-  </si>
-  <si>
-    <t>Varanasi, Índia.</t>
-  </si>
-  <si>
     <t>Nova Zelândia</t>
   </si>
   <si>
-    <t>Chengdu, China.</t>
-  </si>
-  <si>
     <t>Malásia</t>
   </si>
   <si>
-    <t>Sintra, Portugal.</t>
-  </si>
-  <si>
     <t>Coreia do Sul</t>
   </si>
   <si>
-    <t>Florença, Itália.</t>
-  </si>
-  <si>
     <t>Índia</t>
   </si>
   <si>
@@ -1129,42 +1111,18 @@
     <t>Indonésia</t>
   </si>
   <si>
-    <t>Madrid, Espanha.</t>
-  </si>
-  <si>
     <t>Itália</t>
   </si>
   <si>
-    <t>Grécia.</t>
-  </si>
-  <si>
-    <t>Norte do Chipre.</t>
-  </si>
-  <si>
-    <t>Pisa, Itália.</t>
-  </si>
-  <si>
     <t>Cazaquistão</t>
   </si>
   <si>
-    <t>Alexandria, Egito.</t>
-  </si>
-  <si>
-    <t>Historic Jeddah, na Arábia Saudita.</t>
-  </si>
-  <si>
-    <t>Rimini, Itália.</t>
-  </si>
-  <si>
     <t>Hong Kong</t>
   </si>
   <si>
     <t>Polônia</t>
   </si>
   <si>
-    <t>Hanoi, Vietnam.</t>
-  </si>
-  <si>
     <t>Imaterial</t>
   </si>
   <si>
@@ -2618,6 +2576,33 @@
   </si>
   <si>
     <t>engajamento</t>
+  </si>
+  <si>
+    <t>Grécia</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> República Dominicana</t>
+  </si>
+  <si>
+    <t>Arábia Saudita</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chipre</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Espanha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Portugal</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Itália</t>
   </si>
 </sst>
 </file>
@@ -2696,6 +2681,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2987,10 +2976,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="P92" sqref="P92"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="6" max="6" width="62" customWidth="1"/>
     <col min="10" max="10" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -3048,16 +3041,16 @@
         <v>350</v>
       </c>
       <c r="E2" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F2" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="G2" t="s">
-        <v>526</v>
+        <v>511</v>
       </c>
       <c r="H2" t="s">
-        <v>695</v>
+        <v>680</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -3083,16 +3076,16 @@
         <v>350</v>
       </c>
       <c r="E3" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F3" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="G3" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="H3" t="s">
-        <v>696</v>
+        <v>681</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
@@ -3118,16 +3111,16 @@
         <v>350</v>
       </c>
       <c r="E4" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F4" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="G4" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="H4" t="s">
-        <v>697</v>
+        <v>682</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -3153,16 +3146,16 @@
         <v>351</v>
       </c>
       <c r="E5" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F5" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="G5" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
       <c r="H5" t="s">
-        <v>698</v>
+        <v>683</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
@@ -3188,16 +3181,16 @@
         <v>350</v>
       </c>
       <c r="E6" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F6" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="G6" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
       <c r="H6" t="s">
-        <v>699</v>
+        <v>684</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
@@ -3223,16 +3216,16 @@
         <v>350</v>
       </c>
       <c r="E7" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F7" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="G7" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
       <c r="H7" t="s">
-        <v>700</v>
+        <v>685</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
@@ -3258,16 +3251,16 @@
         <v>352</v>
       </c>
       <c r="E8" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F8" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="G8" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
       <c r="H8" t="s">
-        <v>701</v>
+        <v>686</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
@@ -3293,16 +3286,16 @@
         <v>350</v>
       </c>
       <c r="E9" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F9" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="G9" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="H9" t="s">
-        <v>702</v>
+        <v>687</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -3328,16 +3321,16 @@
         <v>350</v>
       </c>
       <c r="E10" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F10" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="G10" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="H10" t="s">
-        <v>703</v>
+        <v>688</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -3363,16 +3356,16 @@
         <v>350</v>
       </c>
       <c r="E11" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F11" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="G11" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="H11" t="s">
-        <v>704</v>
+        <v>689</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -3398,16 +3391,16 @@
         <v>350</v>
       </c>
       <c r="E12" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F12" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="G12" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="H12" t="s">
-        <v>705</v>
+        <v>690</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -3430,19 +3423,19 @@
         <v>2023</v>
       </c>
       <c r="D13" t="s">
-        <v>353</v>
+        <v>851</v>
       </c>
       <c r="E13" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F13" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="G13" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="H13" t="s">
-        <v>706</v>
+        <v>691</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -3465,19 +3458,19 @@
         <v>2023</v>
       </c>
       <c r="D14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E14" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F14" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="G14" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
       <c r="H14" t="s">
-        <v>707</v>
+        <v>692</v>
       </c>
       <c r="J14" t="b">
         <v>0</v>
@@ -3503,16 +3496,16 @@
         <v>350</v>
       </c>
       <c r="E15" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F15" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="G15" t="s">
-        <v>539</v>
+        <v>524</v>
       </c>
       <c r="H15" t="s">
-        <v>708</v>
+        <v>693</v>
       </c>
       <c r="J15" t="b">
         <v>0</v>
@@ -3538,16 +3531,16 @@
         <v>350</v>
       </c>
       <c r="E16" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F16" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="G16" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
       <c r="H16" t="s">
-        <v>709</v>
+        <v>694</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
@@ -3573,16 +3566,16 @@
         <v>350</v>
       </c>
       <c r="E17" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F17" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="G17" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="H17" t="s">
-        <v>710</v>
+        <v>695</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
@@ -3605,19 +3598,19 @@
         <v>2020</v>
       </c>
       <c r="D18" t="s">
-        <v>355</v>
+        <v>852</v>
       </c>
       <c r="E18" t="s">
+        <v>367</v>
+      </c>
+      <c r="F18" t="s">
         <v>382</v>
       </c>
-      <c r="F18" t="s">
-        <v>397</v>
-      </c>
       <c r="G18" t="s">
-        <v>542</v>
+        <v>527</v>
       </c>
       <c r="H18" t="s">
-        <v>711</v>
+        <v>696</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
@@ -3643,16 +3636,16 @@
         <v>350</v>
       </c>
       <c r="E19" t="s">
+        <v>368</v>
+      </c>
+      <c r="F19" t="s">
         <v>383</v>
       </c>
-      <c r="F19" t="s">
-        <v>398</v>
-      </c>
       <c r="G19" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
       <c r="H19" t="s">
-        <v>712</v>
+        <v>697</v>
       </c>
       <c r="J19" t="b">
         <v>0</v>
@@ -3675,19 +3668,19 @@
         <v>2021</v>
       </c>
       <c r="D20" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E20" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F20" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="G20" t="s">
-        <v>544</v>
+        <v>529</v>
       </c>
       <c r="H20" t="s">
-        <v>713</v>
+        <v>698</v>
       </c>
       <c r="J20" t="b">
         <v>0</v>
@@ -3713,16 +3706,16 @@
         <v>350</v>
       </c>
       <c r="E21" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F21" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="G21" t="s">
-        <v>545</v>
+        <v>530</v>
       </c>
       <c r="H21" t="s">
-        <v>714</v>
+        <v>699</v>
       </c>
       <c r="J21" t="b">
         <v>1</v>
@@ -3745,19 +3738,19 @@
         <v>2021</v>
       </c>
       <c r="D22" t="s">
-        <v>357</v>
+        <v>853</v>
       </c>
       <c r="E22" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F22" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="G22" t="s">
-        <v>546</v>
+        <v>531</v>
       </c>
       <c r="H22" t="s">
-        <v>715</v>
+        <v>700</v>
       </c>
       <c r="J22" t="b">
         <v>0</v>
@@ -3783,16 +3776,16 @@
         <v>350</v>
       </c>
       <c r="E23" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F23" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="G23" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="H23" t="s">
-        <v>716</v>
+        <v>701</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
@@ -3818,16 +3811,16 @@
         <v>350</v>
       </c>
       <c r="E24" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F24" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="G24" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
       <c r="H24" t="s">
-        <v>717</v>
+        <v>702</v>
       </c>
       <c r="J24" t="b">
         <v>0</v>
@@ -3853,16 +3846,16 @@
         <v>350</v>
       </c>
       <c r="E25" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F25" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="G25" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
       <c r="H25" t="s">
-        <v>718</v>
+        <v>703</v>
       </c>
       <c r="J25" t="b">
         <v>0</v>
@@ -3888,16 +3881,16 @@
         <v>350</v>
       </c>
       <c r="E26" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F26" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="G26" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
       <c r="H26" t="s">
-        <v>719</v>
+        <v>704</v>
       </c>
       <c r="J26" t="b">
         <v>0</v>
@@ -3923,16 +3916,16 @@
         <v>350</v>
       </c>
       <c r="E27" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F27" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="G27" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="H27" t="s">
-        <v>720</v>
+        <v>705</v>
       </c>
       <c r="J27" t="b">
         <v>1</v>
@@ -3958,16 +3951,16 @@
         <v>350</v>
       </c>
       <c r="E28" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F28" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="G28" t="s">
-        <v>552</v>
+        <v>537</v>
       </c>
       <c r="H28" t="s">
-        <v>721</v>
+        <v>706</v>
       </c>
       <c r="J28" t="b">
         <v>0</v>
@@ -3993,16 +3986,16 @@
         <v>350</v>
       </c>
       <c r="E29" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F29" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="G29" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="H29" t="s">
-        <v>722</v>
+        <v>707</v>
       </c>
       <c r="J29" t="b">
         <v>0</v>
@@ -4028,16 +4021,16 @@
         <v>350</v>
       </c>
       <c r="E30" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F30" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="G30" t="s">
-        <v>554</v>
+        <v>539</v>
       </c>
       <c r="H30" t="s">
-        <v>723</v>
+        <v>708</v>
       </c>
       <c r="J30" t="b">
         <v>1</v>
@@ -4063,16 +4056,16 @@
         <v>358</v>
       </c>
       <c r="E31" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F31" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="G31" t="s">
-        <v>555</v>
+        <v>540</v>
       </c>
       <c r="H31" t="s">
-        <v>724</v>
+        <v>709</v>
       </c>
       <c r="J31" t="b">
         <v>0</v>
@@ -4095,19 +4088,19 @@
         <v>2021</v>
       </c>
       <c r="D32" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E32" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F32" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="G32" t="s">
-        <v>556</v>
+        <v>541</v>
       </c>
       <c r="H32" t="s">
-        <v>725</v>
+        <v>710</v>
       </c>
       <c r="J32" t="b">
         <v>0</v>
@@ -4133,16 +4126,16 @@
         <v>350</v>
       </c>
       <c r="E33" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F33" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="G33" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
       <c r="H33" t="s">
-        <v>726</v>
+        <v>711</v>
       </c>
       <c r="J33" t="b">
         <v>0</v>
@@ -4168,16 +4161,16 @@
         <v>350</v>
       </c>
       <c r="E34" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F34" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="G34" t="s">
-        <v>558</v>
+        <v>543</v>
       </c>
       <c r="H34" t="s">
-        <v>727</v>
+        <v>712</v>
       </c>
       <c r="J34" t="b">
         <v>0</v>
@@ -4203,16 +4196,16 @@
         <v>350</v>
       </c>
       <c r="E35" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F35" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="G35" t="s">
-        <v>559</v>
+        <v>544</v>
       </c>
       <c r="H35" t="s">
-        <v>728</v>
+        <v>713</v>
       </c>
       <c r="J35" t="b">
         <v>0</v>
@@ -4238,16 +4231,16 @@
         <v>350</v>
       </c>
       <c r="E36" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F36" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="G36" t="s">
-        <v>560</v>
+        <v>545</v>
       </c>
       <c r="H36" t="s">
-        <v>729</v>
+        <v>714</v>
       </c>
       <c r="J36" t="b">
         <v>0</v>
@@ -4273,16 +4266,16 @@
         <v>350</v>
       </c>
       <c r="E37" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F37" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="G37" t="s">
-        <v>561</v>
+        <v>546</v>
       </c>
       <c r="H37" t="s">
-        <v>730</v>
+        <v>715</v>
       </c>
       <c r="J37" t="b">
         <v>0</v>
@@ -4308,16 +4301,16 @@
         <v>350</v>
       </c>
       <c r="E38" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F38" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="G38" t="s">
-        <v>562</v>
+        <v>547</v>
       </c>
       <c r="H38" t="s">
-        <v>731</v>
+        <v>716</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
@@ -4343,16 +4336,16 @@
         <v>350</v>
       </c>
       <c r="E39" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F39" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="G39" t="s">
-        <v>563</v>
+        <v>548</v>
       </c>
       <c r="H39" t="s">
-        <v>732</v>
+        <v>717</v>
       </c>
       <c r="J39" t="b">
         <v>0</v>
@@ -4375,22 +4368,22 @@
         <v>2025</v>
       </c>
       <c r="D40" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="E40" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F40" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="G40" t="s">
-        <v>564</v>
+        <v>549</v>
       </c>
       <c r="H40" t="s">
-        <v>733</v>
+        <v>718</v>
       </c>
       <c r="I40" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="J40" t="b">
         <v>0</v>
@@ -4416,16 +4409,16 @@
         <v>350</v>
       </c>
       <c r="E41" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F41" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="G41" t="s">
-        <v>565</v>
+        <v>550</v>
       </c>
       <c r="H41" t="s">
-        <v>734</v>
+        <v>719</v>
       </c>
       <c r="J41" t="b">
         <v>1</v>
@@ -4451,16 +4444,16 @@
         <v>350</v>
       </c>
       <c r="E42" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F42" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="G42" t="s">
-        <v>566</v>
+        <v>551</v>
       </c>
       <c r="H42" t="s">
-        <v>735</v>
+        <v>720</v>
       </c>
       <c r="J42" t="b">
         <v>0</v>
@@ -4483,19 +4476,19 @@
         <v>2024</v>
       </c>
       <c r="D43" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E43" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F43" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="G43" t="s">
-        <v>567</v>
+        <v>552</v>
       </c>
       <c r="H43" t="s">
-        <v>736</v>
+        <v>721</v>
       </c>
       <c r="J43" t="b">
         <v>0</v>
@@ -4521,16 +4514,16 @@
         <v>350</v>
       </c>
       <c r="E44" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F44" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="G44" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="H44" t="s">
-        <v>737</v>
+        <v>722</v>
       </c>
       <c r="J44" t="b">
         <v>1</v>
@@ -4553,19 +4546,19 @@
         <v>2024</v>
       </c>
       <c r="D45" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E45" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F45" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="G45" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="H45" t="s">
-        <v>738</v>
+        <v>723</v>
       </c>
       <c r="J45" t="b">
         <v>0</v>
@@ -4591,16 +4584,16 @@
         <v>350</v>
       </c>
       <c r="E46" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F46" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="G46" t="s">
-        <v>570</v>
+        <v>555</v>
       </c>
       <c r="H46" t="s">
-        <v>739</v>
+        <v>724</v>
       </c>
       <c r="J46" t="b">
         <v>0</v>
@@ -4626,16 +4619,16 @@
         <v>350</v>
       </c>
       <c r="E47" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F47" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="G47" t="s">
-        <v>571</v>
+        <v>556</v>
       </c>
       <c r="H47" t="s">
-        <v>740</v>
+        <v>725</v>
       </c>
       <c r="J47" t="b">
         <v>0</v>
@@ -4661,16 +4654,16 @@
         <v>350</v>
       </c>
       <c r="E48" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F48" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="G48" t="s">
-        <v>572</v>
+        <v>557</v>
       </c>
       <c r="H48" t="s">
-        <v>741</v>
+        <v>726</v>
       </c>
       <c r="J48" t="b">
         <v>0</v>
@@ -4696,16 +4689,16 @@
         <v>350</v>
       </c>
       <c r="E49" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F49" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="G49" t="s">
-        <v>573</v>
+        <v>558</v>
       </c>
       <c r="H49" t="s">
-        <v>742</v>
+        <v>727</v>
       </c>
       <c r="J49" t="b">
         <v>1</v>
@@ -4731,16 +4724,16 @@
         <v>350</v>
       </c>
       <c r="E50" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F50" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="G50" t="s">
-        <v>574</v>
+        <v>559</v>
       </c>
       <c r="H50" t="s">
-        <v>743</v>
+        <v>728</v>
       </c>
       <c r="J50" t="b">
         <v>0</v>
@@ -4766,16 +4759,16 @@
         <v>350</v>
       </c>
       <c r="E51" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F51" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="G51" t="s">
-        <v>575</v>
+        <v>560</v>
       </c>
       <c r="H51" t="s">
-        <v>744</v>
+        <v>729</v>
       </c>
       <c r="J51" t="b">
         <v>0</v>
@@ -4801,16 +4794,16 @@
         <v>350</v>
       </c>
       <c r="E52" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F52" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="G52" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
       <c r="H52" t="s">
-        <v>745</v>
+        <v>730</v>
       </c>
       <c r="J52" t="b">
         <v>0</v>
@@ -4836,16 +4829,16 @@
         <v>350</v>
       </c>
       <c r="E53" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F53" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="G53" t="s">
-        <v>577</v>
+        <v>562</v>
       </c>
       <c r="H53" t="s">
-        <v>746</v>
+        <v>731</v>
       </c>
       <c r="J53" t="b">
         <v>0</v>
@@ -4871,16 +4864,16 @@
         <v>350</v>
       </c>
       <c r="E54" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F54" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="G54" t="s">
-        <v>578</v>
+        <v>563</v>
       </c>
       <c r="H54" t="s">
-        <v>747</v>
+        <v>732</v>
       </c>
       <c r="J54" t="b">
         <v>0</v>
@@ -4906,16 +4899,16 @@
         <v>350</v>
       </c>
       <c r="E55" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F55" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="G55" t="s">
-        <v>579</v>
+        <v>564</v>
       </c>
       <c r="H55" t="s">
-        <v>748</v>
+        <v>733</v>
       </c>
       <c r="J55" t="b">
         <v>0</v>
@@ -4941,16 +4934,16 @@
         <v>350</v>
       </c>
       <c r="E56" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F56" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="G56" t="s">
-        <v>580</v>
+        <v>565</v>
       </c>
       <c r="H56" t="s">
-        <v>749</v>
+        <v>734</v>
       </c>
       <c r="J56" t="b">
         <v>1</v>
@@ -4976,16 +4969,16 @@
         <v>350</v>
       </c>
       <c r="E57" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F57" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="G57" t="s">
-        <v>581</v>
+        <v>566</v>
       </c>
       <c r="H57" t="s">
-        <v>750</v>
+        <v>735</v>
       </c>
       <c r="J57" t="b">
         <v>0</v>
@@ -5008,22 +5001,22 @@
         <v>2021</v>
       </c>
       <c r="D58" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E58" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F58" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="G58" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="H58" t="s">
-        <v>751</v>
+        <v>736</v>
       </c>
       <c r="I58" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="J58" t="b">
         <v>0</v>
@@ -5049,16 +5042,16 @@
         <v>350</v>
       </c>
       <c r="E59" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F59" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="G59" t="s">
-        <v>583</v>
+        <v>568</v>
       </c>
       <c r="H59" t="s">
-        <v>752</v>
+        <v>737</v>
       </c>
       <c r="J59" t="b">
         <v>1</v>
@@ -5084,16 +5077,16 @@
         <v>350</v>
       </c>
       <c r="E60" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F60" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="G60" t="s">
-        <v>584</v>
+        <v>569</v>
       </c>
       <c r="H60" t="s">
-        <v>753</v>
+        <v>738</v>
       </c>
       <c r="J60" t="b">
         <v>0</v>
@@ -5119,16 +5112,16 @@
         <v>350</v>
       </c>
       <c r="E61" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F61" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="G61" t="s">
-        <v>585</v>
+        <v>570</v>
       </c>
       <c r="H61" t="s">
-        <v>754</v>
+        <v>739</v>
       </c>
       <c r="J61" t="b">
         <v>0</v>
@@ -5154,16 +5147,16 @@
         <v>350</v>
       </c>
       <c r="E62" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F62" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="G62" t="s">
-        <v>586</v>
+        <v>571</v>
       </c>
       <c r="H62" t="s">
-        <v>755</v>
+        <v>740</v>
       </c>
       <c r="J62" t="b">
         <v>0</v>
@@ -5189,16 +5182,16 @@
         <v>350</v>
       </c>
       <c r="E63" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F63" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="G63" t="s">
-        <v>587</v>
+        <v>572</v>
       </c>
       <c r="H63" t="s">
-        <v>756</v>
+        <v>741</v>
       </c>
       <c r="J63" t="b">
         <v>0</v>
@@ -5221,19 +5214,19 @@
         <v>2025</v>
       </c>
       <c r="D64" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E64" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F64" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="G64" t="s">
-        <v>588</v>
+        <v>573</v>
       </c>
       <c r="H64" t="s">
-        <v>757</v>
+        <v>742</v>
       </c>
       <c r="J64" t="b">
         <v>0</v>
@@ -5259,16 +5252,16 @@
         <v>350</v>
       </c>
       <c r="E65" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F65" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="G65" t="s">
-        <v>589</v>
+        <v>574</v>
       </c>
       <c r="H65" t="s">
-        <v>758</v>
+        <v>743</v>
       </c>
       <c r="J65" t="b">
         <v>0</v>
@@ -5294,16 +5287,16 @@
         <v>350</v>
       </c>
       <c r="E66" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F66" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="G66" t="s">
-        <v>590</v>
+        <v>575</v>
       </c>
       <c r="H66" t="s">
-        <v>759</v>
+        <v>744</v>
       </c>
       <c r="J66" t="b">
         <v>0</v>
@@ -5329,16 +5322,16 @@
         <v>350</v>
       </c>
       <c r="E67" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F67" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="G67" t="s">
-        <v>591</v>
+        <v>576</v>
       </c>
       <c r="H67" t="s">
-        <v>760</v>
+        <v>745</v>
       </c>
       <c r="J67" t="b">
         <v>0</v>
@@ -5364,16 +5357,16 @@
         <v>350</v>
       </c>
       <c r="E68" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F68" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="G68" t="s">
-        <v>592</v>
+        <v>577</v>
       </c>
       <c r="H68" t="s">
-        <v>761</v>
+        <v>746</v>
       </c>
       <c r="J68" t="b">
         <v>1</v>
@@ -5399,16 +5392,16 @@
         <v>350</v>
       </c>
       <c r="E69" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F69" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="G69" t="s">
-        <v>593</v>
+        <v>578</v>
       </c>
       <c r="H69" t="s">
-        <v>762</v>
+        <v>747</v>
       </c>
       <c r="J69" t="b">
         <v>0</v>
@@ -5434,16 +5427,16 @@
         <v>350</v>
       </c>
       <c r="E70" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F70" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="G70" t="s">
-        <v>594</v>
+        <v>579</v>
       </c>
       <c r="H70" t="s">
-        <v>763</v>
+        <v>748</v>
       </c>
       <c r="J70" t="b">
         <v>0</v>
@@ -5469,16 +5462,16 @@
         <v>350</v>
       </c>
       <c r="E71" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F71" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="G71" t="s">
-        <v>595</v>
+        <v>580</v>
       </c>
       <c r="H71" t="s">
-        <v>764</v>
+        <v>749</v>
       </c>
       <c r="J71" t="b">
         <v>0</v>
@@ -5504,16 +5497,16 @@
         <v>350</v>
       </c>
       <c r="E72" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F72" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="G72" t="s">
-        <v>596</v>
+        <v>581</v>
       </c>
       <c r="H72" t="s">
-        <v>765</v>
+        <v>750</v>
       </c>
       <c r="J72" t="b">
         <v>0</v>
@@ -5539,16 +5532,16 @@
         <v>350</v>
       </c>
       <c r="E73" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F73" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="G73" t="s">
-        <v>597</v>
+        <v>582</v>
       </c>
       <c r="H73" t="s">
-        <v>766</v>
+        <v>751</v>
       </c>
       <c r="J73" t="b">
         <v>0</v>
@@ -5574,16 +5567,16 @@
         <v>350</v>
       </c>
       <c r="E74" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F74" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="G74" t="s">
-        <v>598</v>
+        <v>583</v>
       </c>
       <c r="H74" t="s">
-        <v>767</v>
+        <v>752</v>
       </c>
       <c r="J74" t="b">
         <v>1</v>
@@ -5609,16 +5602,16 @@
         <v>350</v>
       </c>
       <c r="E75" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F75" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="G75" t="s">
-        <v>599</v>
+        <v>584</v>
       </c>
       <c r="H75" t="s">
-        <v>768</v>
+        <v>753</v>
       </c>
       <c r="J75" t="b">
         <v>0</v>
@@ -5644,16 +5637,16 @@
         <v>350</v>
       </c>
       <c r="E76" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F76" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="G76" t="s">
-        <v>600</v>
+        <v>585</v>
       </c>
       <c r="H76" t="s">
-        <v>769</v>
+        <v>754</v>
       </c>
       <c r="J76" t="b">
         <v>0</v>
@@ -5676,19 +5669,19 @@
         <v>2020</v>
       </c>
       <c r="D77" t="s">
-        <v>362</v>
+        <v>857</v>
       </c>
       <c r="E77" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F77" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="G77" t="s">
-        <v>601</v>
+        <v>586</v>
       </c>
       <c r="H77" t="s">
-        <v>770</v>
+        <v>755</v>
       </c>
       <c r="J77" t="b">
         <v>0</v>
@@ -5714,16 +5707,16 @@
         <v>350</v>
       </c>
       <c r="E78" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F78" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="G78" t="s">
-        <v>602</v>
+        <v>587</v>
       </c>
       <c r="H78" t="s">
-        <v>771</v>
+        <v>756</v>
       </c>
       <c r="J78" t="b">
         <v>0</v>
@@ -5749,16 +5742,16 @@
         <v>350</v>
       </c>
       <c r="E79" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F79" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="G79" t="s">
-        <v>603</v>
+        <v>588</v>
       </c>
       <c r="H79" t="s">
-        <v>772</v>
+        <v>757</v>
       </c>
       <c r="J79" t="b">
         <v>0</v>
@@ -5784,16 +5777,16 @@
         <v>350</v>
       </c>
       <c r="E80" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F80" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="G80" t="s">
-        <v>604</v>
+        <v>589</v>
       </c>
       <c r="H80" t="s">
-        <v>773</v>
+        <v>758</v>
       </c>
       <c r="J80" t="b">
         <v>0</v>
@@ -5819,16 +5812,16 @@
         <v>350</v>
       </c>
       <c r="E81" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F81" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="G81" t="s">
-        <v>605</v>
+        <v>590</v>
       </c>
       <c r="H81" t="s">
-        <v>774</v>
+        <v>759</v>
       </c>
       <c r="J81" t="b">
         <v>0</v>
@@ -5854,16 +5847,16 @@
         <v>350</v>
       </c>
       <c r="E82" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F82" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="G82" t="s">
-        <v>606</v>
+        <v>591</v>
       </c>
       <c r="H82" t="s">
-        <v>775</v>
+        <v>760</v>
       </c>
       <c r="J82" t="b">
         <v>0</v>
@@ -5889,16 +5882,16 @@
         <v>350</v>
       </c>
       <c r="E83" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F83" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="G83" t="s">
-        <v>607</v>
+        <v>592</v>
       </c>
       <c r="H83" t="s">
-        <v>776</v>
+        <v>761</v>
       </c>
       <c r="J83" t="b">
         <v>0</v>
@@ -5924,16 +5917,16 @@
         <v>350</v>
       </c>
       <c r="E84" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F84" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="G84" t="s">
-        <v>608</v>
+        <v>593</v>
       </c>
       <c r="H84" t="s">
-        <v>777</v>
+        <v>762</v>
       </c>
       <c r="J84" t="b">
         <v>0</v>
@@ -5959,16 +5952,16 @@
         <v>350</v>
       </c>
       <c r="E85" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F85" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="G85" t="s">
-        <v>609</v>
+        <v>594</v>
       </c>
       <c r="H85" t="s">
-        <v>778</v>
+        <v>763</v>
       </c>
       <c r="J85" t="b">
         <v>0</v>
@@ -5994,16 +5987,16 @@
         <v>350</v>
       </c>
       <c r="E86" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F86" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="G86" t="s">
-        <v>610</v>
+        <v>595</v>
       </c>
       <c r="H86" t="s">
-        <v>779</v>
+        <v>764</v>
       </c>
       <c r="J86" t="b">
         <v>0</v>
@@ -6026,19 +6019,19 @@
         <v>2022</v>
       </c>
       <c r="D87" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E87" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F87" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="G87" t="s">
-        <v>611</v>
+        <v>596</v>
       </c>
       <c r="H87" t="s">
-        <v>780</v>
+        <v>765</v>
       </c>
       <c r="J87" t="b">
         <v>0</v>
@@ -6064,16 +6057,16 @@
         <v>350</v>
       </c>
       <c r="E88" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F88" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="G88" t="s">
-        <v>612</v>
+        <v>597</v>
       </c>
       <c r="H88" t="s">
-        <v>781</v>
+        <v>766</v>
       </c>
       <c r="J88" t="b">
         <v>0</v>
@@ -6099,16 +6092,16 @@
         <v>350</v>
       </c>
       <c r="E89" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F89" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="G89" t="s">
-        <v>613</v>
+        <v>598</v>
       </c>
       <c r="H89" t="s">
-        <v>782</v>
+        <v>767</v>
       </c>
       <c r="J89" t="b">
         <v>0</v>
@@ -6134,16 +6127,16 @@
         <v>350</v>
       </c>
       <c r="E90" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F90" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="G90" t="s">
-        <v>614</v>
+        <v>599</v>
       </c>
       <c r="H90" t="s">
-        <v>783</v>
+        <v>768</v>
       </c>
       <c r="J90" t="b">
         <v>0</v>
@@ -6169,16 +6162,16 @@
         <v>350</v>
       </c>
       <c r="E91" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F91" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="G91" t="s">
-        <v>615</v>
+        <v>600</v>
       </c>
       <c r="H91" t="s">
-        <v>784</v>
+        <v>769</v>
       </c>
       <c r="J91" t="b">
         <v>0</v>
@@ -6204,16 +6197,16 @@
         <v>350</v>
       </c>
       <c r="E92" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F92" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="G92" t="s">
-        <v>616</v>
+        <v>601</v>
       </c>
       <c r="H92" t="s">
-        <v>785</v>
+        <v>770</v>
       </c>
       <c r="J92" t="b">
         <v>0</v>
@@ -6239,16 +6232,16 @@
         <v>350</v>
       </c>
       <c r="E93" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F93" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="G93" t="s">
-        <v>617</v>
+        <v>602</v>
       </c>
       <c r="H93" t="s">
-        <v>786</v>
+        <v>771</v>
       </c>
       <c r="J93" t="b">
         <v>0</v>
@@ -6274,16 +6267,16 @@
         <v>350</v>
       </c>
       <c r="E94" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F94" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="G94" t="s">
-        <v>618</v>
+        <v>603</v>
       </c>
       <c r="H94" t="s">
-        <v>787</v>
+        <v>772</v>
       </c>
       <c r="J94" t="b">
         <v>0</v>
@@ -6309,16 +6302,16 @@
         <v>350</v>
       </c>
       <c r="E95" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F95" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="G95" t="s">
-        <v>619</v>
+        <v>604</v>
       </c>
       <c r="H95" t="s">
-        <v>788</v>
+        <v>773</v>
       </c>
       <c r="J95" t="b">
         <v>0</v>
@@ -6341,19 +6334,19 @@
         <v>2023</v>
       </c>
       <c r="D96" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E96" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F96" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="G96" t="s">
-        <v>620</v>
+        <v>605</v>
       </c>
       <c r="H96" t="s">
-        <v>789</v>
+        <v>774</v>
       </c>
       <c r="J96" t="b">
         <v>0</v>
@@ -6379,16 +6372,16 @@
         <v>350</v>
       </c>
       <c r="E97" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F97" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="G97" t="s">
-        <v>621</v>
+        <v>606</v>
       </c>
       <c r="H97" t="s">
-        <v>790</v>
+        <v>775</v>
       </c>
       <c r="J97" t="b">
         <v>0</v>
@@ -6414,16 +6407,16 @@
         <v>350</v>
       </c>
       <c r="E98" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F98" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="G98" t="s">
-        <v>622</v>
+        <v>607</v>
       </c>
       <c r="H98" t="s">
-        <v>791</v>
+        <v>776</v>
       </c>
       <c r="J98" t="b">
         <v>1</v>
@@ -6449,16 +6442,16 @@
         <v>350</v>
       </c>
       <c r="E99" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F99" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="G99" t="s">
-        <v>623</v>
+        <v>608</v>
       </c>
       <c r="H99" t="s">
-        <v>792</v>
+        <v>777</v>
       </c>
       <c r="J99" t="b">
         <v>0</v>
@@ -6481,19 +6474,19 @@
         <v>2024</v>
       </c>
       <c r="D100" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E100" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F100" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="G100" t="s">
-        <v>624</v>
+        <v>609</v>
       </c>
       <c r="H100" t="s">
-        <v>793</v>
+        <v>778</v>
       </c>
       <c r="J100" t="b">
         <v>0</v>
@@ -6519,16 +6512,16 @@
         <v>350</v>
       </c>
       <c r="E101" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F101" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="G101" t="s">
-        <v>625</v>
+        <v>610</v>
       </c>
       <c r="H101" t="s">
-        <v>794</v>
+        <v>779</v>
       </c>
       <c r="J101" t="b">
         <v>0</v>
@@ -6554,16 +6547,16 @@
         <v>350</v>
       </c>
       <c r="E102" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F102" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
       <c r="G102" t="s">
-        <v>626</v>
+        <v>611</v>
       </c>
       <c r="H102" t="s">
-        <v>795</v>
+        <v>780</v>
       </c>
       <c r="J102" t="b">
         <v>1</v>
@@ -6586,19 +6579,19 @@
         <v>2024</v>
       </c>
       <c r="D103" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E103" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F103" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="G103" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
       <c r="H103" t="s">
-        <v>796</v>
+        <v>781</v>
       </c>
       <c r="J103" t="b">
         <v>0</v>
@@ -6624,16 +6617,16 @@
         <v>350</v>
       </c>
       <c r="E104" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F104" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="G104" t="s">
-        <v>628</v>
+        <v>613</v>
       </c>
       <c r="H104" t="s">
-        <v>797</v>
+        <v>782</v>
       </c>
       <c r="J104" t="b">
         <v>0</v>
@@ -6659,16 +6652,16 @@
         <v>350</v>
       </c>
       <c r="E105" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F105" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="G105" t="s">
-        <v>629</v>
+        <v>614</v>
       </c>
       <c r="H105" t="s">
-        <v>798</v>
+        <v>783</v>
       </c>
       <c r="J105" t="b">
         <v>1</v>
@@ -6691,19 +6684,19 @@
         <v>2025</v>
       </c>
       <c r="D106" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E106" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F106" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="G106" t="s">
-        <v>630</v>
+        <v>615</v>
       </c>
       <c r="H106" t="s">
-        <v>799</v>
+        <v>784</v>
       </c>
       <c r="J106" t="b">
         <v>0</v>
@@ -6726,19 +6719,19 @@
         <v>2024</v>
       </c>
       <c r="D107" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="E107" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F107" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="G107" t="s">
-        <v>631</v>
+        <v>616</v>
       </c>
       <c r="H107" t="s">
-        <v>800</v>
+        <v>785</v>
       </c>
       <c r="J107" t="b">
         <v>0</v>
@@ -6764,16 +6757,16 @@
         <v>350</v>
       </c>
       <c r="E108" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F108" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G108" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
       <c r="H108" t="s">
-        <v>801</v>
+        <v>786</v>
       </c>
       <c r="J108" t="b">
         <v>0</v>
@@ -6796,19 +6789,19 @@
         <v>2023</v>
       </c>
       <c r="D109" t="s">
+        <v>360</v>
+      </c>
+      <c r="E109" t="s">
         <v>367</v>
       </c>
-      <c r="E109" t="s">
-        <v>382</v>
-      </c>
       <c r="F109" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="G109" t="s">
-        <v>633</v>
+        <v>618</v>
       </c>
       <c r="H109" t="s">
-        <v>802</v>
+        <v>787</v>
       </c>
       <c r="J109" t="b">
         <v>0</v>
@@ -6831,19 +6824,19 @@
         <v>2023</v>
       </c>
       <c r="D110" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="E110" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F110" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="G110" t="s">
-        <v>634</v>
+        <v>619</v>
       </c>
       <c r="H110" t="s">
-        <v>803</v>
+        <v>788</v>
       </c>
       <c r="J110" t="b">
         <v>1</v>
@@ -6869,16 +6862,16 @@
         <v>350</v>
       </c>
       <c r="E111" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F111" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="G111" t="s">
-        <v>635</v>
+        <v>620</v>
       </c>
       <c r="H111" t="s">
-        <v>804</v>
+        <v>789</v>
       </c>
       <c r="J111" t="b">
         <v>0</v>
@@ -6904,16 +6897,16 @@
         <v>350</v>
       </c>
       <c r="E112" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F112" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="G112" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="H112" t="s">
-        <v>805</v>
+        <v>790</v>
       </c>
       <c r="J112" t="b">
         <v>0</v>
@@ -6939,16 +6932,16 @@
         <v>350</v>
       </c>
       <c r="E113" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F113" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="G113" t="s">
-        <v>637</v>
+        <v>622</v>
       </c>
       <c r="H113" t="s">
-        <v>806</v>
+        <v>791</v>
       </c>
       <c r="J113" t="b">
         <v>0</v>
@@ -6971,19 +6964,19 @@
         <v>2023</v>
       </c>
       <c r="D114" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E114" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F114" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="G114" t="s">
-        <v>638</v>
+        <v>623</v>
       </c>
       <c r="H114" t="s">
-        <v>807</v>
+        <v>792</v>
       </c>
       <c r="J114" t="b">
         <v>0</v>
@@ -7006,19 +6999,19 @@
         <v>2024</v>
       </c>
       <c r="D115" t="s">
-        <v>369</v>
+        <v>856</v>
       </c>
       <c r="E115" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F115" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="G115" t="s">
-        <v>639</v>
+        <v>624</v>
       </c>
       <c r="H115" t="s">
-        <v>808</v>
+        <v>793</v>
       </c>
       <c r="J115" t="b">
         <v>0</v>
@@ -7044,16 +7037,16 @@
         <v>350</v>
       </c>
       <c r="E116" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F116" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="G116" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
       <c r="H116" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="J116" t="b">
         <v>1</v>
@@ -7079,16 +7072,16 @@
         <v>350</v>
       </c>
       <c r="E117" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F117" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="G117" t="s">
-        <v>641</v>
+        <v>626</v>
       </c>
       <c r="H117" t="s">
-        <v>810</v>
+        <v>795</v>
       </c>
       <c r="J117" t="b">
         <v>0</v>
@@ -7114,16 +7107,16 @@
         <v>350</v>
       </c>
       <c r="E118" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F118" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
       <c r="G118" t="s">
-        <v>642</v>
+        <v>627</v>
       </c>
       <c r="H118" t="s">
-        <v>811</v>
+        <v>796</v>
       </c>
       <c r="J118" t="b">
         <v>0</v>
@@ -7146,19 +7139,19 @@
         <v>2020</v>
       </c>
       <c r="D119" t="s">
+        <v>361</v>
+      </c>
+      <c r="E119" t="s">
         <v>368</v>
       </c>
-      <c r="E119" t="s">
-        <v>383</v>
-      </c>
       <c r="F119" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="G119" t="s">
-        <v>643</v>
+        <v>628</v>
       </c>
       <c r="H119" t="s">
-        <v>812</v>
+        <v>797</v>
       </c>
       <c r="J119" t="b">
         <v>0</v>
@@ -7184,16 +7177,16 @@
         <v>350</v>
       </c>
       <c r="E120" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F120" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="G120" t="s">
-        <v>644</v>
+        <v>629</v>
       </c>
       <c r="H120" t="s">
-        <v>813</v>
+        <v>798</v>
       </c>
       <c r="J120" t="b">
         <v>0</v>
@@ -7216,19 +7209,19 @@
         <v>2020</v>
       </c>
       <c r="D121" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E121" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F121" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="G121" t="s">
-        <v>645</v>
+        <v>630</v>
       </c>
       <c r="H121" t="s">
-        <v>814</v>
+        <v>799</v>
       </c>
       <c r="J121" t="b">
         <v>0</v>
@@ -7251,19 +7244,19 @@
         <v>2024</v>
       </c>
       <c r="D122" t="s">
-        <v>371</v>
+        <v>851</v>
       </c>
       <c r="E122" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F122" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="G122" t="s">
-        <v>646</v>
+        <v>631</v>
       </c>
       <c r="H122" t="s">
-        <v>815</v>
+        <v>800</v>
       </c>
       <c r="J122" t="b">
         <v>1</v>
@@ -7289,16 +7282,16 @@
         <v>350</v>
       </c>
       <c r="E123" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F123" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="G123" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
       <c r="H123" t="s">
-        <v>816</v>
+        <v>801</v>
       </c>
       <c r="J123" t="b">
         <v>0</v>
@@ -7321,22 +7314,22 @@
         <v>2022</v>
       </c>
       <c r="D124" t="s">
-        <v>372</v>
+        <v>855</v>
       </c>
       <c r="E124" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F124" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="G124" t="s">
-        <v>648</v>
+        <v>633</v>
       </c>
       <c r="H124" t="s">
-        <v>817</v>
+        <v>802</v>
       </c>
       <c r="I124" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="J124" t="b">
         <v>0</v>
@@ -7362,16 +7355,16 @@
         <v>350</v>
       </c>
       <c r="E125" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F125" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="G125" t="s">
-        <v>649</v>
+        <v>634</v>
       </c>
       <c r="H125" t="s">
-        <v>818</v>
+        <v>803</v>
       </c>
       <c r="J125" t="b">
         <v>0</v>
@@ -7394,19 +7387,19 @@
         <v>2021</v>
       </c>
       <c r="D126" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E126" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F126" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="G126" t="s">
-        <v>650</v>
+        <v>635</v>
       </c>
       <c r="H126" t="s">
-        <v>819</v>
+        <v>804</v>
       </c>
       <c r="J126" t="b">
         <v>0</v>
@@ -7432,16 +7425,16 @@
         <v>350</v>
       </c>
       <c r="E127" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F127" t="s">
-        <v>491</v>
+        <v>476</v>
       </c>
       <c r="G127" t="s">
-        <v>651</v>
+        <v>636</v>
       </c>
       <c r="H127" t="s">
-        <v>820</v>
+        <v>805</v>
       </c>
       <c r="J127" t="b">
         <v>0</v>
@@ -7467,16 +7460,16 @@
         <v>350</v>
       </c>
       <c r="E128" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F128" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
       <c r="G128" t="s">
-        <v>652</v>
+        <v>637</v>
       </c>
       <c r="H128" t="s">
-        <v>821</v>
+        <v>806</v>
       </c>
       <c r="J128" t="b">
         <v>0</v>
@@ -7499,19 +7492,19 @@
         <v>2020</v>
       </c>
       <c r="D129" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E129" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F129" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="G129" t="s">
-        <v>653</v>
+        <v>638</v>
       </c>
       <c r="H129" t="s">
-        <v>822</v>
+        <v>807</v>
       </c>
       <c r="J129" t="b">
         <v>0</v>
@@ -7534,19 +7527,19 @@
         <v>2024</v>
       </c>
       <c r="D130" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="E130" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F130" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
       <c r="G130" t="s">
-        <v>654</v>
+        <v>639</v>
       </c>
       <c r="H130" t="s">
-        <v>823</v>
+        <v>808</v>
       </c>
       <c r="J130" t="b">
         <v>0</v>
@@ -7572,16 +7565,16 @@
         <v>350</v>
       </c>
       <c r="E131" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F131" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
       <c r="G131" t="s">
-        <v>655</v>
+        <v>640</v>
       </c>
       <c r="H131" t="s">
-        <v>824</v>
+        <v>809</v>
       </c>
       <c r="J131" t="b">
         <v>0</v>
@@ -7607,16 +7600,16 @@
         <v>350</v>
       </c>
       <c r="E132" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F132" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="G132" t="s">
-        <v>656</v>
+        <v>641</v>
       </c>
       <c r="H132" t="s">
-        <v>825</v>
+        <v>810</v>
       </c>
       <c r="J132" t="b">
         <v>0</v>
@@ -7642,16 +7635,16 @@
         <v>350</v>
       </c>
       <c r="E133" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F133" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
       <c r="G133" t="s">
-        <v>657</v>
+        <v>642</v>
       </c>
       <c r="H133" t="s">
-        <v>826</v>
+        <v>811</v>
       </c>
       <c r="J133" t="b">
         <v>0</v>
@@ -7674,19 +7667,19 @@
         <v>2024</v>
       </c>
       <c r="D134" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E134" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F134" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="G134" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
       <c r="H134" t="s">
-        <v>827</v>
+        <v>812</v>
       </c>
       <c r="J134" t="b">
         <v>0</v>
@@ -7712,16 +7705,16 @@
         <v>350</v>
       </c>
       <c r="E135" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F135" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="G135" t="s">
-        <v>659</v>
+        <v>644</v>
       </c>
       <c r="H135" t="s">
-        <v>828</v>
+        <v>813</v>
       </c>
       <c r="J135" t="b">
         <v>0</v>
@@ -7747,19 +7740,19 @@
         <v>350</v>
       </c>
       <c r="E136" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F136" t="s">
-        <v>497</v>
+        <v>482</v>
       </c>
       <c r="G136" t="s">
-        <v>660</v>
+        <v>645</v>
       </c>
       <c r="H136" t="s">
-        <v>829</v>
+        <v>814</v>
       </c>
       <c r="I136" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="J136" t="b">
         <v>0</v>
@@ -7782,19 +7775,19 @@
         <v>2020</v>
       </c>
       <c r="D137" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E137" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F137" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
       <c r="G137" t="s">
-        <v>661</v>
+        <v>646</v>
       </c>
       <c r="H137" t="s">
-        <v>830</v>
+        <v>815</v>
       </c>
       <c r="J137" t="b">
         <v>0</v>
@@ -7817,19 +7810,19 @@
         <v>2024</v>
       </c>
       <c r="D138" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="E138" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F138" t="s">
-        <v>499</v>
+        <v>484</v>
       </c>
       <c r="G138" t="s">
-        <v>662</v>
+        <v>647</v>
       </c>
       <c r="H138" t="s">
-        <v>831</v>
+        <v>816</v>
       </c>
       <c r="J138" t="b">
         <v>0</v>
@@ -7852,19 +7845,19 @@
         <v>2022</v>
       </c>
       <c r="D139" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="E139" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F139" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
       <c r="G139" t="s">
-        <v>663</v>
+        <v>648</v>
       </c>
       <c r="H139" t="s">
-        <v>832</v>
+        <v>817</v>
       </c>
       <c r="J139" t="b">
         <v>0</v>
@@ -7887,19 +7880,19 @@
         <v>2021</v>
       </c>
       <c r="D140" t="s">
-        <v>376</v>
+        <v>854</v>
       </c>
       <c r="E140" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F140" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
       <c r="G140" t="s">
-        <v>664</v>
+        <v>649</v>
       </c>
       <c r="H140" t="s">
-        <v>833</v>
+        <v>818</v>
       </c>
       <c r="J140" t="b">
         <v>0</v>
@@ -7922,19 +7915,19 @@
         <v>2022</v>
       </c>
       <c r="D141" t="s">
-        <v>377</v>
+        <v>859</v>
       </c>
       <c r="E141" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F141" t="s">
-        <v>502</v>
+        <v>487</v>
       </c>
       <c r="G141" t="s">
-        <v>665</v>
+        <v>650</v>
       </c>
       <c r="H141" t="s">
-        <v>834</v>
+        <v>819</v>
       </c>
       <c r="J141" t="b">
         <v>0</v>
@@ -7960,16 +7953,16 @@
         <v>350</v>
       </c>
       <c r="E142" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F142" t="s">
-        <v>503</v>
+        <v>488</v>
       </c>
       <c r="G142" t="s">
-        <v>666</v>
+        <v>651</v>
       </c>
       <c r="H142" t="s">
-        <v>835</v>
+        <v>820</v>
       </c>
       <c r="J142" t="b">
         <v>1</v>
@@ -7995,16 +7988,16 @@
         <v>350</v>
       </c>
       <c r="E143" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F143" t="s">
-        <v>504</v>
+        <v>489</v>
       </c>
       <c r="G143" t="s">
-        <v>667</v>
+        <v>652</v>
       </c>
       <c r="H143" t="s">
-        <v>836</v>
+        <v>821</v>
       </c>
       <c r="J143" t="b">
         <v>1</v>
@@ -8027,19 +8020,19 @@
         <v>2025</v>
       </c>
       <c r="D144" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E144" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F144" t="s">
-        <v>505</v>
+        <v>490</v>
       </c>
       <c r="G144" t="s">
-        <v>668</v>
+        <v>653</v>
       </c>
       <c r="H144" t="s">
-        <v>837</v>
+        <v>822</v>
       </c>
       <c r="J144" t="b">
         <v>0</v>
@@ -8065,19 +8058,19 @@
         <v>350</v>
       </c>
       <c r="E145" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F145" t="s">
-        <v>506</v>
+        <v>491</v>
       </c>
       <c r="G145" t="s">
-        <v>669</v>
+        <v>654</v>
       </c>
       <c r="H145" t="s">
-        <v>838</v>
+        <v>823</v>
       </c>
       <c r="I145" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="J145" t="b">
         <v>0</v>
@@ -8103,16 +8096,16 @@
         <v>350</v>
       </c>
       <c r="E146" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F146" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
       <c r="G146" t="s">
-        <v>670</v>
+        <v>655</v>
       </c>
       <c r="H146" t="s">
-        <v>839</v>
+        <v>824</v>
       </c>
       <c r="J146" t="b">
         <v>0</v>
@@ -8138,16 +8131,16 @@
         <v>350</v>
       </c>
       <c r="E147" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F147" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="G147" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
       <c r="H147" t="s">
-        <v>840</v>
+        <v>825</v>
       </c>
       <c r="J147" t="b">
         <v>0</v>
@@ -8173,16 +8166,16 @@
         <v>350</v>
       </c>
       <c r="E148" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F148" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
       <c r="G148" t="s">
-        <v>672</v>
+        <v>657</v>
       </c>
       <c r="H148" t="s">
-        <v>841</v>
+        <v>826</v>
       </c>
       <c r="J148" t="b">
         <v>0</v>
@@ -8208,16 +8201,16 @@
         <v>350</v>
       </c>
       <c r="E149" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F149" t="s">
-        <v>509</v>
+        <v>494</v>
       </c>
       <c r="G149" t="s">
-        <v>673</v>
+        <v>658</v>
       </c>
       <c r="H149" t="s">
-        <v>842</v>
+        <v>827</v>
       </c>
       <c r="J149" t="b">
         <v>0</v>
@@ -8243,19 +8236,19 @@
         <v>350</v>
       </c>
       <c r="E150" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F150" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
       <c r="G150" t="s">
-        <v>674</v>
+        <v>659</v>
       </c>
       <c r="H150" t="s">
-        <v>843</v>
+        <v>828</v>
       </c>
       <c r="I150" t="s">
-        <v>865</v>
+        <v>850</v>
       </c>
       <c r="J150" t="b">
         <v>0</v>
@@ -8278,19 +8271,19 @@
         <v>2020</v>
       </c>
       <c r="D151" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="E151" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F151" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="G151" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
       <c r="H151" t="s">
-        <v>844</v>
+        <v>829</v>
       </c>
       <c r="J151" t="b">
         <v>0</v>
@@ -8316,16 +8309,16 @@
         <v>350</v>
       </c>
       <c r="E152" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F152" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="G152" t="s">
-        <v>676</v>
+        <v>661</v>
       </c>
       <c r="H152" t="s">
-        <v>845</v>
+        <v>830</v>
       </c>
       <c r="J152" t="b">
         <v>0</v>
@@ -8351,16 +8344,16 @@
         <v>350</v>
       </c>
       <c r="E153" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F153" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
       <c r="G153" t="s">
-        <v>677</v>
+        <v>662</v>
       </c>
       <c r="H153" t="s">
-        <v>846</v>
+        <v>831</v>
       </c>
       <c r="J153" t="b">
         <v>1</v>
@@ -8386,16 +8379,16 @@
         <v>350</v>
       </c>
       <c r="E154" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F154" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
       <c r="G154" t="s">
-        <v>678</v>
+        <v>663</v>
       </c>
       <c r="H154" t="s">
-        <v>847</v>
+        <v>832</v>
       </c>
       <c r="J154" t="b">
         <v>0</v>
@@ -8421,16 +8414,16 @@
         <v>350</v>
       </c>
       <c r="E155" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F155" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
       <c r="G155" t="s">
-        <v>679</v>
+        <v>664</v>
       </c>
       <c r="H155" t="s">
-        <v>848</v>
+        <v>833</v>
       </c>
       <c r="J155" t="b">
         <v>0</v>
@@ -8453,19 +8446,19 @@
         <v>2020</v>
       </c>
       <c r="D156" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="E156" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F156" t="s">
-        <v>514</v>
+        <v>499</v>
       </c>
       <c r="G156" t="s">
-        <v>680</v>
+        <v>665</v>
       </c>
       <c r="H156" t="s">
-        <v>849</v>
+        <v>834</v>
       </c>
       <c r="J156" t="b">
         <v>0</v>
@@ -8491,16 +8484,16 @@
         <v>350</v>
       </c>
       <c r="E157" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F157" t="s">
-        <v>515</v>
+        <v>500</v>
       </c>
       <c r="G157" t="s">
-        <v>681</v>
+        <v>666</v>
       </c>
       <c r="H157" t="s">
-        <v>850</v>
+        <v>835</v>
       </c>
       <c r="J157" t="b">
         <v>0</v>
@@ -8526,16 +8519,16 @@
         <v>350</v>
       </c>
       <c r="E158" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F158" t="s">
-        <v>516</v>
+        <v>501</v>
       </c>
       <c r="G158" t="s">
-        <v>682</v>
+        <v>667</v>
       </c>
       <c r="H158" t="s">
-        <v>851</v>
+        <v>836</v>
       </c>
       <c r="J158" t="b">
         <v>0</v>
@@ -8561,16 +8554,16 @@
         <v>350</v>
       </c>
       <c r="E159" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F159" t="s">
-        <v>517</v>
+        <v>502</v>
       </c>
       <c r="G159" t="s">
-        <v>683</v>
+        <v>668</v>
       </c>
       <c r="H159" t="s">
-        <v>852</v>
+        <v>837</v>
       </c>
       <c r="J159" t="b">
         <v>0</v>
@@ -8593,19 +8586,19 @@
         <v>2023</v>
       </c>
       <c r="D160" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E160" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F160" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
       <c r="G160" t="s">
-        <v>684</v>
+        <v>669</v>
       </c>
       <c r="H160" t="s">
-        <v>853</v>
+        <v>838</v>
       </c>
       <c r="J160" t="b">
         <v>1</v>
@@ -8631,16 +8624,16 @@
         <v>350</v>
       </c>
       <c r="E161" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F161" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="G161" t="s">
-        <v>685</v>
+        <v>670</v>
       </c>
       <c r="H161" t="s">
-        <v>854</v>
+        <v>839</v>
       </c>
       <c r="J161" t="b">
         <v>0</v>
@@ -8666,19 +8659,19 @@
         <v>350</v>
       </c>
       <c r="E162" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F162" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
       <c r="G162" t="s">
-        <v>686</v>
+        <v>671</v>
       </c>
       <c r="H162" t="s">
-        <v>855</v>
+        <v>840</v>
       </c>
       <c r="I162" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="J162" t="b">
         <v>1</v>
@@ -8701,19 +8694,19 @@
         <v>2021</v>
       </c>
       <c r="D163" t="s">
-        <v>380</v>
+        <v>858</v>
       </c>
       <c r="E163" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F163" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="G163" t="s">
-        <v>687</v>
+        <v>672</v>
       </c>
       <c r="H163" t="s">
-        <v>856</v>
+        <v>841</v>
       </c>
       <c r="J163" t="b">
         <v>1</v>
@@ -8736,22 +8729,22 @@
         <v>2024</v>
       </c>
       <c r="D164" t="s">
+        <v>361</v>
+      </c>
+      <c r="E164" t="s">
         <v>368</v>
       </c>
-      <c r="E164" t="s">
-        <v>383</v>
-      </c>
       <c r="F164" t="s">
-        <v>520</v>
+        <v>505</v>
       </c>
       <c r="G164" t="s">
-        <v>688</v>
+        <v>673</v>
       </c>
       <c r="H164" t="s">
-        <v>857</v>
+        <v>842</v>
       </c>
       <c r="I164" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="J164" t="b">
         <v>0</v>
@@ -8777,16 +8770,16 @@
         <v>350</v>
       </c>
       <c r="E165" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F165" t="s">
-        <v>521</v>
+        <v>506</v>
       </c>
       <c r="G165" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="H165" t="s">
-        <v>858</v>
+        <v>843</v>
       </c>
       <c r="J165" t="b">
         <v>0</v>
@@ -8809,19 +8802,19 @@
         <v>2024</v>
       </c>
       <c r="D166" t="s">
+        <v>361</v>
+      </c>
+      <c r="E166" t="s">
         <v>368</v>
       </c>
-      <c r="E166" t="s">
-        <v>383</v>
-      </c>
       <c r="F166" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
       <c r="G166" t="s">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="H166" t="s">
-        <v>859</v>
+        <v>844</v>
       </c>
       <c r="J166" t="b">
         <v>0</v>
@@ -8847,16 +8840,16 @@
         <v>350</v>
       </c>
       <c r="E167" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F167" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
       <c r="G167" t="s">
-        <v>691</v>
+        <v>676</v>
       </c>
       <c r="H167" t="s">
-        <v>860</v>
+        <v>845</v>
       </c>
       <c r="J167" t="b">
         <v>0</v>
@@ -8882,19 +8875,19 @@
         <v>350</v>
       </c>
       <c r="E168" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F168" t="s">
-        <v>524</v>
+        <v>509</v>
       </c>
       <c r="G168" t="s">
-        <v>692</v>
+        <v>677</v>
       </c>
       <c r="H168" t="s">
-        <v>861</v>
+        <v>846</v>
       </c>
       <c r="I168" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="J168" t="b">
         <v>0</v>
@@ -8920,16 +8913,16 @@
         <v>350</v>
       </c>
       <c r="E169" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F169" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="G169" t="s">
-        <v>693</v>
+        <v>678</v>
       </c>
       <c r="H169" t="s">
-        <v>862</v>
+        <v>847</v>
       </c>
       <c r="J169" t="b">
         <v>0</v>
@@ -8955,16 +8948,16 @@
         <v>350</v>
       </c>
       <c r="E170" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F170" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
       <c r="G170" t="s">
-        <v>694</v>
+        <v>679</v>
       </c>
       <c r="H170" t="s">
-        <v>863</v>
+        <v>848</v>
       </c>
       <c r="J170" t="b">
         <v>0</v>

</xml_diff>